<commit_message>
Monitored endpoint already integrated with message
</commit_message>
<xml_diff>
--- a/src/last_values.xlsx
+++ b/src/last_values.xlsx
@@ -1,34 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26529"/>
-  <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://voeazul-my.sharepoint.com/personal/gabriel_bsantos_voeazul_com_br/Documents/Área de Trabalho/Gabriel/ScriptsPy/GitHub/Bc.Watcher.Cron/src/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="14_{06CCC276-A6E7-41CB-B516-71B81144AACE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CA67145A-4485-48B3-8A7A-FF125B3A2FD2}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
-    <t>indicator</t>
+    <t>info</t>
   </si>
   <si>
     <t>value</t>
   </si>
   <si>
-    <t>monitored_total</t>
+    <t>monitored_goods</t>
   </si>
   <si>
     <t>durable_goods</t>
@@ -43,8 +37,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="YYYY-MM-DD HH:MM:SS"/>
+  </numFmts>
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -53,20 +50,7 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <u/>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -91,45 +75,37 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="4" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -143,28 +119,28 @@
         <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="44546A"/>
+        <a:srgbClr val="1F497D"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="E7E6E6"/>
+        <a:srgbClr val="EEECE1"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="4472C4"/>
+        <a:srgbClr val="4F81BD"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="ED7D31"/>
+        <a:srgbClr val="C0504D"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="A5A5A5"/>
+        <a:srgbClr val="9BBB59"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="FFC000"/>
+        <a:srgbClr val="8064A2"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="5B9BD5"/>
+        <a:srgbClr val="4BACC6"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="70AD47"/>
+        <a:srgbClr val="F79646"/>
       </a:accent6>
       <a:hlink>
         <a:srgbClr val="0000FF"/>
@@ -207,7 +183,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -242,7 +217,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -266,6 +240,7 @@
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
+                <a:tint val="15000"/>
                 <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
@@ -276,31 +251,31 @@
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="51000"/>
+                <a:shade val="51000"/>
                 <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="80000">
               <a:schemeClr val="phClr">
-                <a:tint val="15000"/>
+                <a:shade val="93000"/>
                 <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:tint val="94000"/>
+                <a:shade val="94000"/>
                 <a:satMod val="135000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="16200000" scaled="1"/>
+          <a:lin ang="16200000" scaled="0"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
         <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr">
-              <a:shade val="9500"/>
+              <a:shade val="95000"/>
               <a:satMod val="105000"/>
             </a:schemeClr>
           </a:solidFill>
@@ -322,7 +297,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -380,7 +355,7 @@
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:tint val="20000"/>
+                <a:shade val="20000"/>
                 <a:satMod val="255000"/>
               </a:schemeClr>
             </a:gs>
@@ -393,12 +368,13 @@
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
                 <a:satMod val="300000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:tint val="80000"/>
+                <a:shade val="30000"/>
                 <a:satMod val="200000"/>
               </a:schemeClr>
             </a:gs>
@@ -416,60 +392,45 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:F5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.140625" style="1" bestFit="1" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:2">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="3">
-        <v>45078</v>
+      <c r="B2" s="2">
+        <v>45125</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2">
       <c r="A3" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="2"/>
     </row>
-    <row r="4" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2">
       <c r="A4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2">
       <c r="A5" t="s">
         <v>5</v>
       </c>
-      <c r="F5" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <headerFooter>
-    <oddFooter>&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;7&amp;K000000 Este conteúdo e quaisquer informações anexadas a ele são confidenciais e destinados exclusivamente para uso do indivíduo ou pela entidade a quem estão endereçados. Se você recebeu este email por engano, notifique o administrador</oddFooter>
-  </headerFooter>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Implemented the durablegoods endpoint call
</commit_message>
<xml_diff>
--- a/src/last_values.xlsx
+++ b/src/last_values.xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26529"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://voeazul-my.sharepoint.com/personal/gabriel_bsantos_voeazul_com_br/Documents/Área de Trabalho/Gabriel/ScriptsPy/GitHub/Bc.Watcher.Cron/src/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="5" documentId="11_2AA04430D631921FD2FE31D2F8371B86F01040A3" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2F028AD9-318D-4518-9566-CA5EEE9622E8}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -37,11 +43,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="YYYY-MM-DD HH:MM:SS"/>
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
   </numFmts>
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -105,13 +111,21 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -149,7 +163,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -183,6 +197,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -217,9 +232,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -392,14 +408,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.28515625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -407,7 +429,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -415,22 +437,34 @@
         <v>45125</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
+      <c r="B3" s="2">
+        <v>45125</v>
+      </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
+      <c r="B4" s="2">
+        <v>45125</v>
+      </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>5</v>
+      </c>
+      <c r="B5" s="2">
+        <v>45125</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter>
+    <oddFooter>&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;7&amp;K000000 Este conteúdo e quaisquer informações anexadas a ele são confidenciais e destinados exclusivamente para uso do indivíduo ou pela entidade a quem estão endereçados. Se você recebeu este email por engano, notifique o administrador</oddFooter>
+  </headerFooter>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Adjusted the loop and check into xlsx file
</commit_message>
<xml_diff>
--- a/src/last_values.xlsx
+++ b/src/last_values.xlsx
@@ -1,21 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26529"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://voeazul-my.sharepoint.com/personal/gabriel_bsantos_voeazul_com_br/Documents/Área de Trabalho/Gabriel/ScriptsPy/GitHub/Bc.Watcher.Cron/src/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="5" documentId="11_2AA04430D631921FD2FE31D2F8371B86F01040A3" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2F028AD9-318D-4518-9566-CA5EEE9622E8}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -43,11 +37,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
+    <numFmt numFmtId="164" formatCode="YYYY-MM-DD HH:MM:SS"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -111,21 +105,13 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2007 - 2010">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -163,7 +149,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2007 - 2010">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -197,7 +183,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -232,10 +217,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2007 - 2010">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -408,20 +392,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.28515625" bestFit="1" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -429,42 +407,39 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="2">
-        <v>45125</v>
+        <v>45130</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2">
       <c r="A3" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="2">
-        <v>45125</v>
+        <v>45130</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2">
       <c r="A4" t="s">
         <v>4</v>
       </c>
       <c r="B4" s="2">
-        <v>45125</v>
+        <v>45130</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2">
       <c r="A5" t="s">
         <v>5</v>
       </c>
       <c r="B5" s="2">
-        <v>45125</v>
+        <v>45130</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter>
-    <oddFooter>&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;7&amp;K000000 Este conteúdo e quaisquer informações anexadas a ele são confidenciais e destinados exclusivamente para uso do indivíduo ou pela entidade a quem estão endereçados. Se você recebeu este email por engano, notifique o administrador</oddFooter>
-  </headerFooter>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Fixed monitoredData endpoint glitch.
</commit_message>
<xml_diff>
--- a/src/last_values.xlsx
+++ b/src/last_values.xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26529"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://voeazul-my.sharepoint.com/personal/gabriel_bsantos_voeazul_com_br/Documents/Área de Trabalho/Gabriel/ScriptsPy/GitHub/Bc.Watcher.Cron/src/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="3" documentId="11_08AE4430D631921FD2FE31D2F8F8038481335017" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D9367820-D06F-427D-A0FF-980A29D3145E}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -37,11 +43,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="YYYY-MM-DD HH:MM:SS"/>
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
   </numFmts>
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -105,13 +111,21 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -149,7 +163,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -183,6 +197,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -217,9 +232,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -392,14 +408,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="18.28515625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -407,15 +428,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="2">
-        <v>45130</v>
+        <v>45078</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -423,7 +444,7 @@
         <v>45130</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -431,7 +452,7 @@
         <v>45130</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -441,5 +462,8 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter>
+    <oddFooter>&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;7&amp;K000000 Este conteúdo e quaisquer informações anexadas a ele são confidenciais e destinados exclusivamente para uso do indivíduo ou pela entidade a quem estão endereçados. Se você recebeu este email por engano, notifique o administrador</oddFooter>
+  </headerFooter>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added mean calculations to the sendMessage
</commit_message>
<xml_diff>
--- a/src/last_values.xlsx
+++ b/src/last_values.xlsx
@@ -1,21 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26529"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://voeazul-my.sharepoint.com/personal/gabriel_bsantos_voeazul_com_br/Documents/Área de Trabalho/Gabriel/ScriptsPy/GitHub/Bc.Watcher.Cron/src/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="11_08AE4430D631921FD2FE31D2F8F8038481335017" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D9367820-D06F-427D-A0FF-980A29D3145E}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -43,11 +37,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
+    <numFmt numFmtId="164" formatCode="YYYY-MM-DD HH:MM:SS"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -111,21 +105,13 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2007 - 2010">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -163,7 +149,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2007 - 2010">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -197,7 +183,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -232,10 +217,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2007 - 2010">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -408,19 +392,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="18.28515625" bestFit="1" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -428,7 +407,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -436,7 +415,7 @@
         <v>45078</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -444,7 +423,7 @@
         <v>45130</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -452,7 +431,7 @@
         <v>45130</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -462,8 +441,5 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter>
-    <oddFooter>&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;7&amp;K000000 Este conteúdo e quaisquer informações anexadas a ele são confidenciais e destinados exclusivamente para uso do indivíduo ou pela entidade a quem estão endereçados. Se você recebeu este email por engano, notifique o administrador</oddFooter>
-  </headerFooter>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Implemented the get record link
</commit_message>
<xml_diff>
--- a/src/last_values.xlsx
+++ b/src/last_values.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>info</t>
   </si>
@@ -32,6 +32,9 @@
   </si>
   <si>
     <t>services</t>
+  </si>
+  <si>
+    <t>record_date</t>
   </si>
 </sst>
 </file>
@@ -393,7 +396,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -420,7 +423,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="2">
-        <v>45130</v>
+        <v>45078</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -428,7 +431,7 @@
         <v>4</v>
       </c>
       <c r="B4" s="2">
-        <v>45130</v>
+        <v>45078</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -436,7 +439,15 @@
         <v>5</v>
       </c>
       <c r="B5" s="2">
-        <v>45130</v>
+        <v>45078</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="2">
+        <v>45146</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Move the record to be the first to broadcast
</commit_message>
<xml_diff>
--- a/src/last_values.xlsx
+++ b/src/last_values.xlsx
@@ -1,69 +1,40 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
-  <workbookPr defaultThemeVersion="124226"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <workbookPr/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
+  <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
-  <si>
-    <t>info</t>
-  </si>
-  <si>
-    <t>value</t>
-  </si>
-  <si>
-    <t>monitored_goods</t>
-  </si>
-  <si>
-    <t>durable_goods</t>
-  </si>
-  <si>
-    <t>non_durable_goods</t>
-  </si>
-  <si>
-    <t>services</t>
-  </si>
-  <si>
-    <t>record_date</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="YYYY-MM-DD HH:MM:SS"/>
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="yyyy-mm-dd h:mm:ss"/>
+    <numFmt numFmtId="165" formatCode="YYYY-MM-DD HH:MM:SS"/>
   </numFmts>
   <fonts count="2">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
+      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -78,36 +49,94 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -395,62 +424,82 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>info</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>value</t>
+        </is>
       </c>
     </row>
-    <row r="2" spans="1:2">
-      <c r="A2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="2">
-        <v>45078</v>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>monitored_goods</t>
+        </is>
+      </c>
+      <c r="B2" s="2" t="n">
+        <v>45200</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
-      <c r="A3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="2">
-        <v>45078</v>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>durable_goods</t>
+        </is>
+      </c>
+      <c r="B3" s="2" t="n">
+        <v>45200</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
-      <c r="A4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="2">
-        <v>45078</v>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>non_durable_goods</t>
+        </is>
+      </c>
+      <c r="B4" s="2" t="n">
+        <v>45200</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
-      <c r="A5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" s="2">
-        <v>45078</v>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>services</t>
+        </is>
+      </c>
+      <c r="B5" s="2" t="n">
+        <v>45200</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
-      <c r="A6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" s="2">
-        <v>45146</v>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>record_date</t>
+        </is>
+      </c>
+      <c r="B6" s="2" t="n">
+        <v>45237</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>